<commit_message>
add logs file for hours tracking
</commit_message>
<xml_diff>
--- a/Yazan-DTT-Assessment-Hour-Log.xlsx
+++ b/Yazan-DTT-Assessment-Hour-Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <r>
       <rPr>
@@ -69,6 +69,63 @@
   </si>
   <si>
     <t>Fix some dependencies issues and implement the design guidline.</t>
+  </si>
+  <si>
+    <t>Implement first user story</t>
+  </si>
+  <si>
+    <t>Create reusable components and implement the navigation.</t>
+  </si>
+  <si>
+    <t>Create Scss BEM structure</t>
+  </si>
+  <si>
+    <t>28/08/2025</t>
+  </si>
+  <si>
+    <t>restructured the css classes to be more optimized scss.</t>
+  </si>
+  <si>
+    <t>Implement user story 2,3,4</t>
+  </si>
+  <si>
+    <t>Implement user stories and refactore some code to be scaled</t>
+  </si>
+  <si>
+    <t>Implement user story 5</t>
+  </si>
+  <si>
+    <t>Integrate the API for details page together with some functionalities.</t>
+  </si>
+  <si>
+    <t>Implement user story 6, 7</t>
+  </si>
+  <si>
+    <t>29/08/2025</t>
+  </si>
+  <si>
+    <t>Integrate edit and create apis and design the form user hapy flow.</t>
+  </si>
+  <si>
+    <t>Implement user story 8, 9</t>
+  </si>
+  <si>
+    <t>Create delete logic and create reusable comosables to be reused cross components</t>
+  </si>
+  <si>
+    <t>Refactor and simplify ideas for performance</t>
+  </si>
+  <si>
+    <t>Removed some ideas that added complaxity to the images loads</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add some bonus points pages </t>
+  </si>
+  <si>
+    <t>30/08/2025</t>
+  </si>
+  <si>
+    <t>Implemented some extra points, pages as my list, favorites and history.</t>
   </si>
   <si>
     <t>Total amount of hours</t>
@@ -733,66 +790,130 @@
       <c r="F5" s="10"/>
     </row>
     <row r="6" ht="16.5" customHeight="1">
-      <c r="A6" s="17"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
+      <c r="A6" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>13</v>
+      </c>
       <c r="E6" s="15"/>
       <c r="F6" s="10"/>
     </row>
     <row r="7" ht="16.5" customHeight="1">
-      <c r="A7" s="17"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
+      <c r="A7" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>16</v>
+      </c>
       <c r="E7" s="15"/>
       <c r="F7" s="10"/>
     </row>
     <row r="8" ht="16.5" customHeight="1">
-      <c r="A8" s="17"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
+      <c r="A8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="12">
+        <v>4.0</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>18</v>
+      </c>
       <c r="E8" s="15"/>
       <c r="F8" s="10"/>
     </row>
     <row r="9" ht="16.5" customHeight="1">
-      <c r="A9" s="17"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
+      <c r="A9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>20</v>
+      </c>
       <c r="E9" s="15"/>
       <c r="F9" s="10"/>
     </row>
     <row r="10" ht="16.5" customHeight="1">
-      <c r="A10" s="17"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
+      <c r="A10" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="12">
+        <v>3.0</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>23</v>
+      </c>
       <c r="E10" s="15"/>
       <c r="F10" s="10"/>
     </row>
     <row r="11" ht="16.5" customHeight="1">
-      <c r="A11" s="17"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="19"/>
+      <c r="A11" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>25</v>
+      </c>
       <c r="E11" s="15"/>
       <c r="F11" s="10"/>
     </row>
     <row r="12" ht="16.5" customHeight="1">
-      <c r="A12" s="17"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="19"/>
+      <c r="A12" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="12">
+        <v>2.0</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="E12" s="15"/>
       <c r="F12" s="10"/>
     </row>
     <row r="13" ht="16.5" customHeight="1">
-      <c r="A13" s="17"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="19"/>
+      <c r="A13" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="12">
+        <v>1.0</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>30</v>
+      </c>
       <c r="E13" s="15"/>
       <c r="F13" s="10"/>
     </row>
@@ -926,11 +1047,11 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="23" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="B30" s="24">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>

</xml_diff>